<commit_message>
Imerção Alura Python: Aplicando função la,bda para criar lógica para a coluna Status
</commit_message>
<xml_diff>
--- a/Alura_Python/Projeto_imerção_Python/acoes_pura.xlsx
+++ b/Alura_Python/Projeto_imerção_Python/acoes_pura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\GitHub\Python\Alura_Python\Projeto_imerção_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17510F6D-7ACB-4F87-B116-B4D28C46BE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9327BAAA-5A7F-4B0E-926A-3EC881302A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34785" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -6024,7 +6024,7 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>